<commit_message>
Add code for callSummaries aggregate calculations; fixed error on division by zero for revenueChange
</commit_message>
<xml_diff>
--- a/FieldCategorisation.xlsx
+++ b/FieldCategorisation.xlsx
@@ -564,8 +564,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -589,7 +589,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -645,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -659,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -673,7 +673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -687,7 +687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -701,7 +701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -715,7 +715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -729,7 +729,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -771,7 +771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -785,7 +785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -799,7 +799,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -827,7 +827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -841,7 +841,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" hidden="1">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -855,7 +855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" hidden="1">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -869,7 +869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" hidden="1">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -883,7 +883,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -897,7 +897,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -911,7 +911,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" hidden="1">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -939,7 +939,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" hidden="1">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -953,7 +953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" hidden="1">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -967,7 +967,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" hidden="1">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -981,7 +981,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1013,7 +1013,7 @@
   <autoFilter ref="A1:D31">
     <filterColumn colId="0">
       <filters>
-        <filter val="bills"/>
+        <filter val="summaries"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Adding final fixes and tidy up
</commit_message>
<xml_diff>
--- a/FieldCategorisation.xlsx
+++ b/FieldCategorisation.xlsx
@@ -561,16 +561,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" bestFit="1" customWidth="1"/>
   </cols>
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -617,7 +617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -631,7 +631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -743,7 +743,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -757,7 +757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -813,7 +813,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -841,7 +841,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -855,7 +855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -869,7 +869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -911,7 +911,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -925,7 +925,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -939,7 +939,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -953,7 +953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -967,7 +967,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -995,7 +995,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1011,11 +1011,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D31">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="summaries"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="0"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>